<commit_message>
cleaning for level 2 creation
</commit_message>
<xml_diff>
--- a/System/system_management.xlsx
+++ b/System/system_management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC8C6EF-20C7-457D-B2D1-A99EFFCFF241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77F9201-F49F-47B1-BDE8-585CFBF39B3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -417,7 +417,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
asignamos WoS en base a clase social
</commit_message>
<xml_diff>
--- a/System/system_management.xlsx
+++ b/System/system_management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77F9201-F49F-47B1-BDE8-585CFBF39B3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0134692D-FD07-47A6-8D64-23C9A21D5042}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>archetypes</t>
   </si>
@@ -97,14 +97,37 @@
   </si>
   <si>
     <t>Entertainment</t>
+  </si>
+  <si>
+    <t>stats</t>
+  </si>
+  <si>
+    <t>synpop</t>
+  </si>
+  <si>
+    <t>trans</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>building</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,8 +155,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,39 +438,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -460,10 +490,13 @@
       <c r="E2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -477,10 +510,13 @@
       <c r="E3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -494,10 +530,13 @@
       <c r="E4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -509,7 +548,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -520,7 +562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -531,7 +573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -542,7 +584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -553,7 +595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -565,6 +607,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="F2:F4">
+    <sortCondition ref="F2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>